<commit_message>
clean company names of accents and group, then analyse
</commit_message>
<xml_diff>
--- a/input-data/lseg_columns_needed.xlsx
+++ b/input-data/lseg_columns_needed.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="636" documentId="8_{59694D10-1ADE-A449-AC98-835B8DC94CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{022950AF-DB0E-8A46-B1F3-31DA5AD47960}"/>
   <bookViews>
-    <workbookView xWindow="-4020" yWindow="-18920" windowWidth="31900" windowHeight="16480" xr2:uid="{AD20F702-6B9F-7F4A-9CFC-34D2E60F3FF2}"/>
+    <workbookView xWindow="11020" yWindow="2640" windowWidth="18380" windowHeight="16480" xr2:uid="{AD20F702-6B9F-7F4A-9CFC-34D2E60F3FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1325,7 +1325,7 @@
   <dimension ref="A1:G172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4287,17 +4287,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="193858b9-a7e5-46a0-a17e-3020908dcb20">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="74939e57-9d5a-4a0e-92b8-734534a31947" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100782D128FB6981541A51099910CFC1E4B" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f74102cfec586183eca87f50d115a912">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="193858b9-a7e5-46a0-a17e-3020908dcb20" xmlns:ns3="74939e57-9d5a-4a0e-92b8-734534a31947" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="80a57a212c8dac7c54b70a8786012a0b" ns2:_="" ns3:_="">
     <xsd:import namespace="193858b9-a7e5-46a0-a17e-3020908dcb20"/>
@@ -4546,6 +4535,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="193858b9-a7e5-46a0-a17e-3020908dcb20">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="74939e57-9d5a-4a0e-92b8-734534a31947" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4556,23 +4556,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F3FA12-1D2A-49BC-ACD8-7A41D6FBC181}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="193858b9-a7e5-46a0-a17e-3020908dcb20"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="74939e57-9d5a-4a0e-92b8-734534a31947"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{642F7E26-E2A6-4CAB-8C0E-88FD4AF632AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4591,6 +4574,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F3FA12-1D2A-49BC-ACD8-7A41D6FBC181}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="74939e57-9d5a-4a0e-92b8-734534a31947"/>
+    <ds:schemaRef ds:uri="193858b9-a7e5-46a0-a17e-3020908dcb20"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{440E0154-4747-4FA3-8651-122E7C61EF0D}">
   <ds:schemaRefs>

</xml_diff>